<commit_message>
updated table to 6th orders (13 coeffs)
</commit_message>
<xml_diff>
--- a/ComparisonTable.xlsx
+++ b/ComparisonTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{144D3124-2766-493D-8E6A-B351A5308816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DD0771B-32EE-41D3-AB01-27A9D868C6CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2039CBC-118C-445F-AA3C-064BAB4B5E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3495" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +18,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -108,6 +106,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1923,6 +1924,606 @@
         <a:xfrm>
           <a:off x="1771650" y="21526500"/>
           <a:ext cx="5334000" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4D003F-5E6E-4C1E-B253-CD5C6A76173B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1790700" y="25584150"/>
+          <a:ext cx="5619749" cy="5067300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00AB7249-D2A0-41C8-802E-B678B6F98519}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7353301" y="25584150"/>
+          <a:ext cx="5524500" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5505451</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4428184B-6A63-4D40-ABA3-B4FB29704CCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12877801" y="25584150"/>
+          <a:ext cx="5505450" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B6F1106-66D1-4313-B7D8-391E97671BA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18402301" y="25584150"/>
+          <a:ext cx="5543550" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B774DA5-323B-4159-9869-A59B77EE16F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23926801" y="25584150"/>
+          <a:ext cx="5543550" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD4EC78-09F7-4E77-9032-0E227F839ABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29451301" y="25584150"/>
+          <a:ext cx="5543550" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5486401</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5000000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C36DFA-EEE0-4060-A7A6-A66685B7E6EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="25584150"/>
+          <a:ext cx="5486400" cy="5000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDDF50FD-2C27-484D-BF31-57808754F767}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="1238250"/>
+          <a:ext cx="5505450" cy="4057650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486EB9E0-E5DD-4482-B2C1-A7979F48F279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="5295900"/>
+          <a:ext cx="5505450" cy="4129087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297DA0DB-0FEE-4D50-8B70-208AEE3027DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="13411200"/>
+          <a:ext cx="5524500" cy="4143375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5486401</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA960184-2DE2-4675-A923-288637119419}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="17468850"/>
+          <a:ext cx="5486400" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F011A0A5-E0C6-43E8-83E5-387A22A5C63D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34975801" y="21526500"/>
+          <a:ext cx="5505450" cy="4129087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2197,35 +2798,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="8" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="8" width="80.6640625" customWidth="1"/>
+    <col min="9" max="9" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36">
+    <row r="3" spans="1:9" ht="36.6" x14ac:dyDescent="0.7">
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="31.5">
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -2244,38 +2846,64 @@
       <c r="H4" s="1">
         <v>11</v>
       </c>
+      <c r="I4" s="1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="5" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
+      <c r="H5" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="6" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
+      <c r="H6" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="7" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
+      <c r="H7" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="8" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>7</v>
       </c>
+      <c r="H8" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="9" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>9</v>
       </c>
+      <c r="H9" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="320.10000000000002" customHeight="1">
+    <row r="10" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>11</v>
+      </c>
+      <c r="H10" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="394.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2286,12 +2914,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2479,19 +3104,45 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38B5A086-C995-40AA-BBD0-CC00F31EAE10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C957C660-A9EC-416D-B80A-E70548D9CE86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635E68C0-511C-41B1-9EB2-243C23A954A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635E68C0-511C-41B1-9EB2-243C23A954A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4db6b2d7-13c9-4786-99f0-2b48490331aa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C957C660-A9EC-416D-B80A-E70548D9CE86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38B5A086-C995-40AA-BBD0-CC00F31EAE10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>